<commit_message>
added user input for v_c
</commit_message>
<xml_diff>
--- a/example/input_1_Mast.xlsx
+++ b/example/input_1_Mast.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dokumente\MARS\mars-softwaredemonstrator\tests\input_file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dokumente\MARS\mars-softwaredemonstrator\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -239,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0">
+    <comment ref="B15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -276,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0">
+    <comment ref="B17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
+    <comment ref="B18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0">
+    <comment ref="B19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -324,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -340,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -356,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -372,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -388,7 +388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
+    <comment ref="B24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -401,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B23" authorId="0" shapeId="0">
+    <comment ref="B25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -414,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B24" authorId="0" shapeId="0">
+    <comment ref="B26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -428,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0" shapeId="0">
+    <comment ref="B27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -444,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0" shapeId="0">
+    <comment ref="B28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -457,7 +457,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B27" authorId="0" shapeId="0">
+    <comment ref="B29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -473,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="B30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -486,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0">
+    <comment ref="B31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -499,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0">
+    <comment ref="B34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -513,7 +513,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="0" shapeId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -526,7 +526,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0" shapeId="0">
+    <comment ref="B36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -639,7 +639,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="176">
   <si>
     <t>0.3</t>
   </si>
@@ -1159,6 +1159,18 @@
   <si>
     <t>http://mars-demonstrator.de/about/</t>
   </si>
+  <si>
+    <t>Wheel_Relative_Number_of_Rolling_Contacts v_c</t>
+  </si>
+  <si>
+    <t>Rail_Relative_Number_of_Rolling_Contacts v_c</t>
+  </si>
+  <si>
+    <t>v_c_w</t>
+  </si>
+  <si>
+    <t>v_c_r</t>
+  </si>
 </sst>
 </file>
 
@@ -1531,7 +1543,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1675,6 +1687,9 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1703,6 +1718,46 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2219,46 +2274,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2359,13 +2374,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>854075</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>110358</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2397,13 +2412,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1308100</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>71125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3932239</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>87795</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2435,13 +2450,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4723924</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>37361</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>704111</xdr:colOff>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>165101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2559,63 +2574,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="railmaterials" displayName="railmaterials" ref="A2:I9" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" headerRowCellStyle="Gut">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="railmaterials" displayName="railmaterials" ref="A2:I9" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" headerRowCellStyle="Gut">
   <autoFilter ref="A2:I9"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Name" dataDxfId="32"/>
-    <tableColumn id="2" name="Norm" dataDxfId="31"/>
-    <tableColumn id="3" name="Material Number" dataDxfId="30"/>
-    <tableColumn id="4" name="Hardened Surface (yes = 1, no = 0) " dataDxfId="29"/>
-    <tableColumn id="5" name="Yield Point at the Depth of Maximum Shear _x000a_ f_y [N/mm²]" dataDxfId="28"/>
-    <tableColumn id="6" name="Unit-Conform Hardness_x000a_HB" dataDxfId="27"/>
-    <tableColumn id="7" name="E-Moduleus [N/mm²]" dataDxfId="26"/>
-    <tableColumn id="8" name="Radial-Strain-Coefficient-v" dataDxfId="25"/>
-    <tableColumn id="9" name="Depth-Of-Achieved-Hardeness-Surface z [mm]" dataDxfId="24"/>
+    <tableColumn id="1" name="Name" dataDxfId="36"/>
+    <tableColumn id="2" name="Norm" dataDxfId="35"/>
+    <tableColumn id="3" name="Material Number" dataDxfId="34"/>
+    <tableColumn id="4" name="Hardened Surface (yes = 1, no = 0) " dataDxfId="33"/>
+    <tableColumn id="5" name="Yield Point at the Depth of Maximum Shear _x000a_ f_y [N/mm²]" dataDxfId="32"/>
+    <tableColumn id="6" name="Unit-Conform Hardness_x000a_HB" dataDxfId="31"/>
+    <tableColumn id="7" name="E-Moduleus [N/mm²]" dataDxfId="30"/>
+    <tableColumn id="8" name="Radial-Strain-Coefficient-v" dataDxfId="29"/>
+    <tableColumn id="9" name="Depth-Of-Achieved-Hardeness-Surface z [mm]" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="wheelmaterials4" displayName="wheelmaterials4" ref="A2:I10" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowCellStyle="Gut">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="wheelmaterials4" displayName="wheelmaterials4" ref="A2:I10" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="Gut">
   <autoFilter ref="A2:I10"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Name" dataDxfId="21"/>
-    <tableColumn id="2" name="Norm" dataDxfId="20"/>
-    <tableColumn id="3" name="Material Number" dataDxfId="19"/>
-    <tableColumn id="4" name="Hardened Surface (yes = 1, no = 0) " dataDxfId="18"/>
-    <tableColumn id="9" name="Yield Point at the Depth of Maximum Shear _x000a_ f_y [N/mm²]" dataDxfId="17"/>
-    <tableColumn id="5" name="Unit-Conform Hardness_x000a_HB" dataDxfId="16"/>
-    <tableColumn id="6" name="E-Moduleus [N/mm²]" dataDxfId="15"/>
-    <tableColumn id="7" name="Radial-Strain-Coefficient-v" dataDxfId="14"/>
-    <tableColumn id="8" name="Depth-Of-Achieved-Hardeness-Surface _x000a_z [mm]" dataDxfId="13"/>
+    <tableColumn id="1" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Norm" dataDxfId="24"/>
+    <tableColumn id="3" name="Material Number" dataDxfId="23"/>
+    <tableColumn id="4" name="Hardened Surface (yes = 1, no = 0) " dataDxfId="22"/>
+    <tableColumn id="9" name="Yield Point at the Depth of Maximum Shear _x000a_ f_y [N/mm²]" dataDxfId="21"/>
+    <tableColumn id="5" name="Unit-Conform Hardness_x000a_HB" dataDxfId="20"/>
+    <tableColumn id="6" name="E-Moduleus [N/mm²]" dataDxfId="19"/>
+    <tableColumn id="7" name="Radial-Strain-Coefficient-v" dataDxfId="18"/>
+    <tableColumn id="8" name="Depth-Of-Achieved-Hardeness-Surface _x000a_z [mm]" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="wheelgeometries" displayName="wheelgeometries" ref="A2:E21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="wheelgeometries" displayName="wheelgeometries" ref="A2:E21" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A2:E21"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="10"/>
-    <tableColumn id="2" name="Load-bearing-Width b_w [mm]" dataDxfId="9"/>
-    <tableColumn id="3" name="Second-Wheel-Radius r_k [mm]" dataDxfId="8"/>
-    <tableColumn id="4" name="Edge-Radius r_3 [mm]" dataDxfId="7"/>
-    <tableColumn id="5" name="Diameter D_w" dataDxfId="6"/>
+    <tableColumn id="1" name="Name" dataDxfId="14"/>
+    <tableColumn id="2" name="Load-bearing-Width b_w [mm]" dataDxfId="13"/>
+    <tableColumn id="3" name="Second-Wheel-Radius r_k [mm]" dataDxfId="12"/>
+    <tableColumn id="4" name="Edge-Radius r_3 [mm]" dataDxfId="11"/>
+    <tableColumn id="5" name="Diameter D_w" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="railgeometries" displayName="railgeometries" ref="A2:D10" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="railgeometries" displayName="railgeometries" ref="A2:D10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A2:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="3"/>
-    <tableColumn id="2" name="Load-bearing-Width b_r [mm]" dataDxfId="2"/>
-    <tableColumn id="3" name="Rail-Surface-Radius r_k [mm]" dataDxfId="1"/>
-    <tableColumn id="4" name="Edge-Radius r_3 [mm]" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="7"/>
+    <tableColumn id="2" name="Load-bearing-Width b_r [mm]" dataDxfId="6"/>
+    <tableColumn id="3" name="Rail-Surface-Radius r_k [mm]" dataDxfId="5"/>
+    <tableColumn id="4" name="Edge-Radius r_3 [mm]" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4497,16 +4512,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FD1895"/>
+  <dimension ref="A1:FD1897"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="84.85546875" customWidth="1"/>
-    <col min="3" max="3" width="0.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.140625" customWidth="1"/>
@@ -4514,7 +4529,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>72</v>
       </c>
       <c r="B1" s="40" t="s">
@@ -4688,7 +4703,7 @@
       <c r="FD1" s="40"/>
     </row>
     <row r="2" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
+      <c r="A2" s="51"/>
       <c r="B2" s="47" t="s">
         <v>170</v>
       </c>
@@ -4860,7 +4875,7 @@
       <c r="FD2" s="47"/>
     </row>
     <row r="3" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="7" t="s">
         <v>78</v>
       </c>
@@ -5032,7 +5047,7 @@
       <c r="FD3" s="7"/>
     </row>
     <row r="4" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="47" t="s">
         <v>77</v>
       </c>
@@ -5204,7 +5219,7 @@
       <c r="FD4" s="47"/>
     </row>
     <row r="5" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="7" t="s">
         <v>89</v>
       </c>
@@ -5376,7 +5391,7 @@
       <c r="FD5" s="7"/>
     </row>
     <row r="6" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="47" t="s">
         <v>123</v>
       </c>
@@ -5548,7 +5563,7 @@
       <c r="FD6" s="47"/>
     </row>
     <row r="7" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="7" t="s">
         <v>107</v>
       </c>
@@ -5720,7 +5735,7 @@
       <c r="FD7" s="7"/>
     </row>
     <row r="8" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="47" t="s">
         <v>90</v>
       </c>
@@ -5892,7 +5907,7 @@
       <c r="FD8" s="47"/>
     </row>
     <row r="9" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="7" t="s">
         <v>132</v>
       </c>
@@ -6064,7 +6079,7 @@
       <c r="FD9" s="7"/>
     </row>
     <row r="10" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="47" t="s">
         <v>133</v>
       </c>
@@ -6236,7 +6251,7 @@
       <c r="FD10" s="47"/>
     </row>
     <row r="11" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="7" t="s">
         <v>128</v>
       </c>
@@ -6408,7 +6423,7 @@
       <c r="FD11" s="7"/>
     </row>
     <row r="12" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="47" t="s">
         <v>129</v>
       </c>
@@ -6579,29 +6594,27 @@
       <c r="FC12" s="47"/>
       <c r="FD12" s="47"/>
     </row>
-    <row r="13" spans="1:160" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
-        <v>125</v>
-      </c>
+    <row r="13" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="49"/>
       <c r="B13" s="7" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="46">
-        <v>24.9397924881983</v>
-      </c>
-      <c r="E13" s="46">
-        <v>29.846033506748501</v>
-      </c>
-      <c r="F13" s="46">
-        <v>29.846033506748501</v>
-      </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
+        <v>174</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>8</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -6754,26 +6767,26 @@
       <c r="FD13" s="7"/>
     </row>
     <row r="14" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="47" t="s">
-        <v>110</v>
+        <v>173</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="48">
-        <v>0.397534327540081</v>
-      </c>
-      <c r="E14" s="48">
-        <v>0.38745672969163403</v>
-      </c>
-      <c r="F14" s="48">
-        <v>0.38745672969163403</v>
-      </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
+        <v>175</v>
+      </c>
+      <c r="D14" s="47">
+        <v>0</v>
+      </c>
+      <c r="E14" s="47">
+        <v>0</v>
+      </c>
+      <c r="F14" s="47">
+        <v>0</v>
+      </c>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
       <c r="K14" s="47"/>
       <c r="L14" s="47"/>
       <c r="M14" s="47"/>
@@ -6925,22 +6938,24 @@
       <c r="FC14" s="47"/>
       <c r="FD14" s="47"/>
     </row>
-    <row r="15" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
+    <row r="15" spans="1:160" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54" t="s">
+        <v>125</v>
+      </c>
       <c r="B15" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="46">
-        <v>310.53423258511901</v>
+        <v>24.9397924881983</v>
       </c>
       <c r="E15" s="46">
-        <v>311.82631932244198</v>
+        <v>29.846033506748501</v>
       </c>
       <c r="F15" s="46">
-        <v>311.82631932244198</v>
+        <v>29.846033506748501</v>
       </c>
       <c r="G15" s="46"/>
       <c r="H15" s="46"/>
@@ -7098,21 +7113,21 @@
       <c r="FD15" s="7"/>
     </row>
     <row r="16" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="48">
-        <v>0.2</v>
+        <v>0.397534327540081</v>
       </c>
       <c r="E16" s="48">
-        <v>0.27896020164795099</v>
+        <v>0.38745672969163403</v>
       </c>
       <c r="F16" s="48">
-        <v>0.27896020164795099</v>
+        <v>0.38745672969163403</v>
       </c>
       <c r="G16" s="48"/>
       <c r="H16" s="48"/>
@@ -7270,21 +7285,21 @@
       <c r="FD16" s="47"/>
     </row>
     <row r="17" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="46">
-        <v>9592.8821295104699</v>
+        <v>310.53423258511901</v>
       </c>
       <c r="E17" s="46">
-        <v>13728.6250951821</v>
+        <v>311.82631932244198</v>
       </c>
       <c r="F17" s="46">
-        <v>13728.6250951821</v>
+        <v>311.82631932244198</v>
       </c>
       <c r="G17" s="46"/>
       <c r="H17" s="46"/>
@@ -7442,21 +7457,21 @@
       <c r="FD17" s="7"/>
     </row>
     <row r="18" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="47" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="48">
-        <v>6.9859353305379797</v>
+        <v>0.2</v>
       </c>
       <c r="E18" s="48">
-        <v>4.8667038063889603</v>
+        <v>0.27896020164795099</v>
       </c>
       <c r="F18" s="48">
-        <v>4.8667038063889603</v>
+        <v>0.27896020164795099</v>
       </c>
       <c r="G18" s="48"/>
       <c r="H18" s="48"/>
@@ -7614,21 +7629,21 @@
       <c r="FD18" s="47"/>
     </row>
     <row r="19" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
+      <c r="A19" s="55"/>
       <c r="B19" s="7" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" s="46">
-        <v>0.36032232455732299</v>
+        <v>9592.8821295104699</v>
       </c>
       <c r="E19" s="46">
-        <v>0.43263553136410199</v>
+        <v>13728.6250951821</v>
       </c>
       <c r="F19" s="46">
-        <v>0.43263553136410199</v>
+        <v>13728.6250951821</v>
       </c>
       <c r="G19" s="46"/>
       <c r="H19" s="46"/>
@@ -7786,21 +7801,21 @@
       <c r="FD19" s="7"/>
     </row>
     <row r="20" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
+      <c r="A20" s="55"/>
       <c r="B20" s="47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20" s="48">
-        <v>235.360704664796</v>
+        <v>6.9859353305379797</v>
       </c>
       <c r="E20" s="48">
-        <v>208.806759033595</v>
+        <v>4.8667038063889603</v>
       </c>
       <c r="F20" s="48">
-        <v>208.806759033595</v>
+        <v>4.8667038063889603</v>
       </c>
       <c r="G20" s="48"/>
       <c r="H20" s="48"/>
@@ -7958,21 +7973,21 @@
       <c r="FD20" s="47"/>
     </row>
     <row r="21" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="54"/>
+      <c r="A21" s="55"/>
       <c r="B21" s="7" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="46">
-        <v>3620.8448324163101</v>
+        <v>0.36032232455732299</v>
       </c>
       <c r="E21" s="46">
-        <v>2311.15858694705</v>
+        <v>0.43263553136410199</v>
       </c>
       <c r="F21" s="46">
-        <v>2311.15858694705</v>
+        <v>0.43263553136410199</v>
       </c>
       <c r="G21" s="46"/>
       <c r="H21" s="46"/>
@@ -8130,21 +8145,21 @@
       <c r="FD21" s="7"/>
     </row>
     <row r="22" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="47" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="48">
-        <v>1.13373577673032</v>
+        <v>235.360704664796</v>
       </c>
       <c r="E22" s="48">
-        <v>2.4258179969420199</v>
+        <v>208.806759033595</v>
       </c>
       <c r="F22" s="48">
-        <v>2.4258179969420199</v>
+        <v>208.806759033595</v>
       </c>
       <c r="G22" s="48"/>
       <c r="H22" s="48"/>
@@ -8302,21 +8317,21 @@
       <c r="FD22" s="47"/>
     </row>
     <row r="23" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
+      <c r="A23" s="55"/>
       <c r="B23" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D23" s="46">
-        <v>0.67575877439752896</v>
+        <v>3620.8448324163101</v>
       </c>
       <c r="E23" s="46">
-        <v>0.51712000434017502</v>
+        <v>2311.15858694705</v>
       </c>
       <c r="F23" s="46">
-        <v>0.51712000434017502</v>
+        <v>2311.15858694705</v>
       </c>
       <c r="G23" s="46"/>
       <c r="H23" s="46"/>
@@ -8474,21 +8489,21 @@
       <c r="FD23" s="7"/>
     </row>
     <row r="24" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
+      <c r="A24" s="55"/>
       <c r="B24" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24" s="48">
-        <v>3.8387980542432998</v>
+        <v>1.13373577673032</v>
       </c>
       <c r="E24" s="48">
-        <v>1.8776339003870799</v>
+        <v>2.4258179969420199</v>
       </c>
       <c r="F24" s="48">
-        <v>1.8776339003870799</v>
+        <v>2.4258179969420199</v>
       </c>
       <c r="G24" s="48"/>
       <c r="H24" s="48"/>
@@ -8646,21 +8661,21 @@
       <c r="FD24" s="47"/>
     </row>
     <row r="25" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
-      <c r="B25" s="41" t="s">
-        <v>127</v>
+      <c r="A25" s="55"/>
+      <c r="B25" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D25" s="46">
-        <v>1.2</v>
+        <v>0.67575877439752896</v>
       </c>
       <c r="E25" s="46">
-        <v>3.2</v>
+        <v>0.51712000434017502</v>
       </c>
       <c r="F25" s="46">
-        <v>3.1</v>
+        <v>0.51712000434017502</v>
       </c>
       <c r="G25" s="46"/>
       <c r="H25" s="46"/>
@@ -8818,21 +8833,21 @@
       <c r="FD25" s="7"/>
     </row>
     <row r="26" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
+      <c r="A26" s="55"/>
       <c r="B26" s="47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" s="48">
-        <v>2351.0358557609202</v>
+        <v>3.8387980542432998</v>
       </c>
       <c r="E26" s="48">
-        <v>2600</v>
+        <v>1.8776339003870799</v>
       </c>
       <c r="F26" s="48">
-        <v>2600</v>
+        <v>1.8776339003870799</v>
       </c>
       <c r="G26" s="48"/>
       <c r="H26" s="48"/>
@@ -8990,21 +9005,21 @@
       <c r="FD26" s="47"/>
     </row>
     <row r="27" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="7" t="s">
-        <v>86</v>
+      <c r="A27" s="55"/>
+      <c r="B27" s="41" t="s">
+        <v>127</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D27" s="46">
-        <v>479.56427978543297</v>
+        <v>1.2</v>
       </c>
       <c r="E27" s="46">
-        <v>342.07526272382</v>
+        <v>3.2</v>
       </c>
       <c r="F27" s="46">
-        <v>342.07526272382</v>
+        <v>3.1</v>
       </c>
       <c r="G27" s="46"/>
       <c r="H27" s="46"/>
@@ -9162,21 +9177,21 @@
       <c r="FD27" s="7"/>
     </row>
     <row r="28" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
+      <c r="A28" s="55"/>
       <c r="B28" s="47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D28" s="48">
-        <v>1.5209241133552001</v>
+        <v>2351.0358557609202</v>
       </c>
       <c r="E28" s="48">
-        <v>1.4611356146706</v>
+        <v>2600</v>
       </c>
       <c r="F28" s="48">
-        <v>1.4611356146706</v>
+        <v>2600</v>
       </c>
       <c r="G28" s="48"/>
       <c r="H28" s="48"/>
@@ -9334,21 +9349,21 @@
       <c r="FD28" s="47"/>
     </row>
     <row r="29" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
+      <c r="A29" s="55"/>
       <c r="B29" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D29" s="46">
-        <v>148.023377589456</v>
+        <v>479.56427978543297</v>
       </c>
       <c r="E29" s="46">
-        <v>90</v>
+        <v>342.07526272382</v>
       </c>
       <c r="F29" s="46">
-        <v>90</v>
+        <v>342.07526272382</v>
       </c>
       <c r="G29" s="46"/>
       <c r="H29" s="46"/>
@@ -9506,26 +9521,26 @@
       <c r="FD29" s="7"/>
     </row>
     <row r="30" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
+      <c r="A30" s="55"/>
       <c r="B30" s="47" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="47">
-        <v>4000000</v>
-      </c>
-      <c r="E30" s="47">
-        <v>4000000</v>
-      </c>
-      <c r="F30" s="47">
-        <v>4000000</v>
-      </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+        <v>53</v>
+      </c>
+      <c r="D30" s="48">
+        <v>1.5209241133552001</v>
+      </c>
+      <c r="E30" s="48">
+        <v>1.4611356146706</v>
+      </c>
+      <c r="F30" s="48">
+        <v>1.4611356146706</v>
+      </c>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
       <c r="K30" s="47"/>
       <c r="L30" s="47"/>
       <c r="M30" s="47"/>
@@ -9678,26 +9693,26 @@
       <c r="FD30" s="47"/>
     </row>
     <row r="31" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
+      <c r="A31" s="55"/>
       <c r="B31" s="7" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="7">
-        <v>12000000</v>
-      </c>
-      <c r="E31" s="7">
-        <v>13000000</v>
-      </c>
-      <c r="F31" s="7">
-        <v>13000000</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="D31" s="46">
+        <v>148.023377589456</v>
+      </c>
+      <c r="E31" s="46">
+        <v>90</v>
+      </c>
+      <c r="F31" s="46">
+        <v>90</v>
+      </c>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
@@ -9849,22 +9864,22 @@
       <c r="FC31" s="7"/>
       <c r="FD31" s="7"/>
     </row>
-    <row r="32" spans="1:160" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
       <c r="B32" s="47" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D32" s="47">
-        <v>1</v>
+        <v>4000000</v>
       </c>
       <c r="E32" s="47">
-        <v>2</v>
+        <v>4000000</v>
       </c>
       <c r="F32" s="47">
-        <v>4</v>
+        <v>4000000</v>
       </c>
       <c r="G32" s="47"/>
       <c r="H32" s="47"/>
@@ -10022,1282 +10037,1620 @@
       <c r="FD32" s="47"/>
     </row>
     <row r="33" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="55"/>
+      <c r="B33" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="7">
+        <v>12000000</v>
+      </c>
+      <c r="E33" s="7">
+        <v>13000000</v>
+      </c>
+      <c r="F33" s="7">
+        <v>13000000</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="7"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7"/>
+      <c r="AK33" s="7"/>
+      <c r="AL33" s="7"/>
+      <c r="AM33" s="7"/>
+      <c r="AN33" s="7"/>
+      <c r="AO33" s="7"/>
+      <c r="AP33" s="7"/>
+      <c r="AQ33" s="7"/>
+      <c r="AR33" s="7"/>
+      <c r="AS33" s="7"/>
+      <c r="AT33" s="7"/>
+      <c r="AU33" s="7"/>
+      <c r="AV33" s="7"/>
+      <c r="AW33" s="7"/>
+      <c r="AX33" s="7"/>
+      <c r="AY33" s="7"/>
+      <c r="AZ33" s="7"/>
+      <c r="BA33" s="7"/>
+      <c r="BB33" s="7"/>
+      <c r="BC33" s="7"/>
+      <c r="BD33" s="7"/>
+      <c r="BE33" s="7"/>
+      <c r="BF33" s="7"/>
+      <c r="BG33" s="7"/>
+      <c r="BH33" s="7"/>
+      <c r="BI33" s="7"/>
+      <c r="BJ33" s="7"/>
+      <c r="BK33" s="7"/>
+      <c r="BL33" s="7"/>
+      <c r="BM33" s="7"/>
+      <c r="BN33" s="7"/>
+      <c r="BO33" s="7"/>
+      <c r="BP33" s="7"/>
+      <c r="BQ33" s="7"/>
+      <c r="BR33" s="7"/>
+      <c r="BS33" s="7"/>
+      <c r="BT33" s="7"/>
+      <c r="BU33" s="7"/>
+      <c r="BV33" s="7"/>
+      <c r="BW33" s="7"/>
+      <c r="BX33" s="7"/>
+      <c r="BY33" s="7"/>
+      <c r="BZ33" s="7"/>
+      <c r="CA33" s="7"/>
+      <c r="CB33" s="7"/>
+      <c r="CC33" s="7"/>
+      <c r="CD33" s="7"/>
+      <c r="CE33" s="7"/>
+      <c r="CF33" s="7"/>
+      <c r="CG33" s="7"/>
+      <c r="CH33" s="7"/>
+      <c r="CI33" s="7"/>
+      <c r="CJ33" s="7"/>
+      <c r="CK33" s="7"/>
+      <c r="CL33" s="7"/>
+      <c r="CM33" s="7"/>
+      <c r="CN33" s="7"/>
+      <c r="CO33" s="7"/>
+      <c r="CP33" s="7"/>
+      <c r="CQ33" s="7"/>
+      <c r="CR33" s="7"/>
+      <c r="CS33" s="7"/>
+      <c r="CT33" s="7"/>
+      <c r="CU33" s="7"/>
+      <c r="CV33" s="7"/>
+      <c r="CW33" s="7"/>
+      <c r="CX33" s="7"/>
+      <c r="CY33" s="7"/>
+      <c r="CZ33" s="7"/>
+      <c r="DA33" s="7"/>
+      <c r="DB33" s="7"/>
+      <c r="DC33" s="7"/>
+      <c r="DD33" s="7"/>
+      <c r="DE33" s="7"/>
+      <c r="DF33" s="7"/>
+      <c r="DG33" s="7"/>
+      <c r="DH33" s="7"/>
+      <c r="DI33" s="7"/>
+      <c r="DJ33" s="7"/>
+      <c r="DK33" s="7"/>
+      <c r="DL33" s="7"/>
+      <c r="DM33" s="7"/>
+      <c r="DN33" s="7"/>
+      <c r="DO33" s="7"/>
+      <c r="DP33" s="7"/>
+      <c r="DQ33" s="7"/>
+      <c r="DR33" s="7"/>
+      <c r="DS33" s="7"/>
+      <c r="DT33" s="7"/>
+      <c r="DU33" s="7"/>
+      <c r="DV33" s="7"/>
+      <c r="DW33" s="7"/>
+      <c r="DX33" s="7"/>
+      <c r="DY33" s="7"/>
+      <c r="DZ33" s="7"/>
+      <c r="EA33" s="7"/>
+      <c r="EB33" s="7"/>
+      <c r="EC33" s="7"/>
+      <c r="ED33" s="7"/>
+      <c r="EE33" s="7"/>
+      <c r="EF33" s="7"/>
+      <c r="EG33" s="7"/>
+      <c r="EH33" s="7"/>
+      <c r="EI33" s="7"/>
+      <c r="EJ33" s="7"/>
+      <c r="EK33" s="7"/>
+      <c r="EL33" s="7"/>
+      <c r="EM33" s="7"/>
+      <c r="EN33" s="7"/>
+      <c r="EO33" s="7"/>
+      <c r="EP33" s="7"/>
+      <c r="EQ33" s="7"/>
+      <c r="ER33" s="7"/>
+      <c r="ES33" s="7"/>
+      <c r="ET33" s="7"/>
+      <c r="EU33" s="7"/>
+      <c r="EV33" s="7"/>
+      <c r="EW33" s="7"/>
+      <c r="EX33" s="7"/>
+      <c r="EY33" s="7"/>
+      <c r="EZ33" s="7"/>
+      <c r="FA33" s="7"/>
+      <c r="FB33" s="7"/>
+      <c r="FC33" s="7"/>
+      <c r="FD33" s="7"/>
+    </row>
+    <row r="34" spans="1:160" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="56"/>
+      <c r="B34" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="47">
+        <v>1</v>
+      </c>
+      <c r="E34" s="47">
+        <v>2</v>
+      </c>
+      <c r="F34" s="47">
+        <v>4</v>
+      </c>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
+      <c r="Q34" s="47"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="47"/>
+      <c r="T34" s="47"/>
+      <c r="U34" s="47"/>
+      <c r="V34" s="47"/>
+      <c r="W34" s="47"/>
+      <c r="X34" s="47"/>
+      <c r="Y34" s="47"/>
+      <c r="Z34" s="47"/>
+      <c r="AA34" s="47"/>
+      <c r="AB34" s="47"/>
+      <c r="AC34" s="47"/>
+      <c r="AD34" s="47"/>
+      <c r="AE34" s="47"/>
+      <c r="AF34" s="47"/>
+      <c r="AG34" s="47"/>
+      <c r="AH34" s="47"/>
+      <c r="AI34" s="47"/>
+      <c r="AJ34" s="47"/>
+      <c r="AK34" s="47"/>
+      <c r="AL34" s="47"/>
+      <c r="AM34" s="47"/>
+      <c r="AN34" s="47"/>
+      <c r="AO34" s="47"/>
+      <c r="AP34" s="47"/>
+      <c r="AQ34" s="47"/>
+      <c r="AR34" s="47"/>
+      <c r="AS34" s="47"/>
+      <c r="AT34" s="47"/>
+      <c r="AU34" s="47"/>
+      <c r="AV34" s="47"/>
+      <c r="AW34" s="47"/>
+      <c r="AX34" s="47"/>
+      <c r="AY34" s="47"/>
+      <c r="AZ34" s="47"/>
+      <c r="BA34" s="47"/>
+      <c r="BB34" s="47"/>
+      <c r="BC34" s="47"/>
+      <c r="BD34" s="47"/>
+      <c r="BE34" s="47"/>
+      <c r="BF34" s="47"/>
+      <c r="BG34" s="47"/>
+      <c r="BH34" s="47"/>
+      <c r="BI34" s="47"/>
+      <c r="BJ34" s="47"/>
+      <c r="BK34" s="47"/>
+      <c r="BL34" s="47"/>
+      <c r="BM34" s="47"/>
+      <c r="BN34" s="47"/>
+      <c r="BO34" s="47"/>
+      <c r="BP34" s="47"/>
+      <c r="BQ34" s="47"/>
+      <c r="BR34" s="47"/>
+      <c r="BS34" s="47"/>
+      <c r="BT34" s="47"/>
+      <c r="BU34" s="47"/>
+      <c r="BV34" s="47"/>
+      <c r="BW34" s="47"/>
+      <c r="BX34" s="47"/>
+      <c r="BY34" s="47"/>
+      <c r="BZ34" s="47"/>
+      <c r="CA34" s="47"/>
+      <c r="CB34" s="47"/>
+      <c r="CC34" s="47"/>
+      <c r="CD34" s="47"/>
+      <c r="CE34" s="47"/>
+      <c r="CF34" s="47"/>
+      <c r="CG34" s="47"/>
+      <c r="CH34" s="47"/>
+      <c r="CI34" s="47"/>
+      <c r="CJ34" s="47"/>
+      <c r="CK34" s="47"/>
+      <c r="CL34" s="47"/>
+      <c r="CM34" s="47"/>
+      <c r="CN34" s="47"/>
+      <c r="CO34" s="47"/>
+      <c r="CP34" s="47"/>
+      <c r="CQ34" s="47"/>
+      <c r="CR34" s="47"/>
+      <c r="CS34" s="47"/>
+      <c r="CT34" s="47"/>
+      <c r="CU34" s="47"/>
+      <c r="CV34" s="47"/>
+      <c r="CW34" s="47"/>
+      <c r="CX34" s="47"/>
+      <c r="CY34" s="47"/>
+      <c r="CZ34" s="47"/>
+      <c r="DA34" s="47"/>
+      <c r="DB34" s="47"/>
+      <c r="DC34" s="47"/>
+      <c r="DD34" s="47"/>
+      <c r="DE34" s="47"/>
+      <c r="DF34" s="47"/>
+      <c r="DG34" s="47"/>
+      <c r="DH34" s="47"/>
+      <c r="DI34" s="47"/>
+      <c r="DJ34" s="47"/>
+      <c r="DK34" s="47"/>
+      <c r="DL34" s="47"/>
+      <c r="DM34" s="47"/>
+      <c r="DN34" s="47"/>
+      <c r="DO34" s="47"/>
+      <c r="DP34" s="47"/>
+      <c r="DQ34" s="47"/>
+      <c r="DR34" s="47"/>
+      <c r="DS34" s="47"/>
+      <c r="DT34" s="47"/>
+      <c r="DU34" s="47"/>
+      <c r="DV34" s="47"/>
+      <c r="DW34" s="47"/>
+      <c r="DX34" s="47"/>
+      <c r="DY34" s="47"/>
+      <c r="DZ34" s="47"/>
+      <c r="EA34" s="47"/>
+      <c r="EB34" s="47"/>
+      <c r="EC34" s="47"/>
+      <c r="ED34" s="47"/>
+      <c r="EE34" s="47"/>
+      <c r="EF34" s="47"/>
+      <c r="EG34" s="47"/>
+      <c r="EH34" s="47"/>
+      <c r="EI34" s="47"/>
+      <c r="EJ34" s="47"/>
+      <c r="EK34" s="47"/>
+      <c r="EL34" s="47"/>
+      <c r="EM34" s="47"/>
+      <c r="EN34" s="47"/>
+      <c r="EO34" s="47"/>
+      <c r="EP34" s="47"/>
+      <c r="EQ34" s="47"/>
+      <c r="ER34" s="47"/>
+      <c r="ES34" s="47"/>
+      <c r="ET34" s="47"/>
+      <c r="EU34" s="47"/>
+      <c r="EV34" s="47"/>
+      <c r="EW34" s="47"/>
+      <c r="EX34" s="47"/>
+      <c r="EY34" s="47"/>
+      <c r="EZ34" s="47"/>
+      <c r="FA34" s="47"/>
+      <c r="FB34" s="47"/>
+      <c r="FC34" s="47"/>
+      <c r="FD34" s="47"/>
+    </row>
+    <row r="35" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="37" t="str">
-        <f>IF((D13-0.8)*D15 &gt;D17, "ERROR", "OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="E33" s="37" t="str">
-        <f t="shared" ref="E33:O33" si="0">IF((E13-0.8)*E15 &gt;E17, "ERROR", "OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="F33" s="37" t="str">
+      <c r="C35" s="36"/>
+      <c r="D35" s="37" t="str">
+        <f>IF((D15-0.8)*D17 &gt;D19, "ERROR", "OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="E35" s="37" t="str">
+        <f t="shared" ref="E35:O35" si="0">IF((E15-0.8)*E17 &gt;E19, "ERROR", "OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="F35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="G33" s="37" t="str">
+      <c r="G35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="H33" s="37" t="str">
+      <c r="H35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="I33" s="37" t="str">
+      <c r="I35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="J33" s="37" t="str">
+      <c r="J35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="K33" s="37" t="str">
+      <c r="K35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="L33" s="37" t="str">
+      <c r="L35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="M33" s="37" t="str">
+      <c r="M35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="N33" s="37" t="str">
+      <c r="N35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="O33" s="37" t="str">
+      <c r="O35" s="37" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="P33" s="37" t="str">
-        <f t="shared" ref="P33:CA33" si="1">IF((P13-0.8)*P15 &gt;P17, "ERROR", "OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="Q33" s="37" t="str">
+      <c r="P35" s="37" t="str">
+        <f t="shared" ref="P35:CA35" si="1">IF((P15-0.8)*P17 &gt;P19, "ERROR", "OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="Q35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="R33" s="37" t="str">
+      <c r="R35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="S33" s="37" t="str">
+      <c r="S35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="T33" s="37" t="str">
+      <c r="T35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="U33" s="37" t="str">
+      <c r="U35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="V33" s="37" t="str">
+      <c r="V35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="W33" s="37" t="str">
+      <c r="W35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="X33" s="37" t="str">
+      <c r="X35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="Y33" s="37" t="str">
+      <c r="Y35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="Z33" s="37" t="str">
+      <c r="Z35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AA33" s="37" t="str">
+      <c r="AA35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AB33" s="37" t="str">
+      <c r="AB35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AC33" s="37" t="str">
+      <c r="AC35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AD33" s="37" t="str">
+      <c r="AD35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AE33" s="37" t="str">
+      <c r="AE35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AF33" s="37" t="str">
+      <c r="AF35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AG33" s="37" t="str">
+      <c r="AG35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AH33" s="37" t="str">
+      <c r="AH35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AI33" s="37" t="str">
+      <c r="AI35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AJ33" s="37" t="str">
+      <c r="AJ35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AK33" s="37" t="str">
+      <c r="AK35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AL33" s="37" t="str">
+      <c r="AL35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AM33" s="37" t="str">
+      <c r="AM35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AN33" s="37" t="str">
+      <c r="AN35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AO33" s="37" t="str">
+      <c r="AO35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AP33" s="37" t="str">
+      <c r="AP35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AQ33" s="37" t="str">
+      <c r="AQ35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AR33" s="37" t="str">
+      <c r="AR35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AS33" s="37" t="str">
+      <c r="AS35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AT33" s="37" t="str">
+      <c r="AT35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AU33" s="37" t="str">
+      <c r="AU35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AV33" s="37" t="str">
+      <c r="AV35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AW33" s="37" t="str">
+      <c r="AW35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AX33" s="37" t="str">
+      <c r="AX35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AY33" s="37" t="str">
+      <c r="AY35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="AZ33" s="37" t="str">
+      <c r="AZ35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BA33" s="37" t="str">
+      <c r="BA35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BB33" s="37" t="str">
+      <c r="BB35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BC33" s="37" t="str">
+      <c r="BC35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BD33" s="37" t="str">
+      <c r="BD35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BE33" s="37" t="str">
+      <c r="BE35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BF33" s="37" t="str">
+      <c r="BF35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BG33" s="37" t="str">
+      <c r="BG35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BH33" s="37" t="str">
+      <c r="BH35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BI33" s="37" t="str">
+      <c r="BI35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BJ33" s="37" t="str">
+      <c r="BJ35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BK33" s="37" t="str">
+      <c r="BK35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BL33" s="37" t="str">
+      <c r="BL35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BM33" s="37" t="str">
+      <c r="BM35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BN33" s="37" t="str">
+      <c r="BN35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BO33" s="37" t="str">
+      <c r="BO35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BP33" s="37" t="str">
+      <c r="BP35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BQ33" s="37" t="str">
+      <c r="BQ35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BR33" s="37" t="str">
+      <c r="BR35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BS33" s="37" t="str">
+      <c r="BS35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BT33" s="37" t="str">
+      <c r="BT35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BU33" s="37" t="str">
+      <c r="BU35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BV33" s="37" t="str">
+      <c r="BV35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BW33" s="37" t="str">
+      <c r="BW35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BX33" s="37" t="str">
+      <c r="BX35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BY33" s="37" t="str">
+      <c r="BY35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="BZ33" s="37" t="str">
+      <c r="BZ35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="CA33" s="37" t="str">
+      <c r="CA35" s="37" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-      <c r="CB33" s="37" t="str">
-        <f t="shared" ref="CB33:EM33" si="2">IF((CB13-0.8)*CB15 &gt;CB17, "ERROR", "OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="CC33" s="37" t="str">
+      <c r="CB35" s="37" t="str">
+        <f t="shared" ref="CB35:EM35" si="2">IF((CB15-0.8)*CB17 &gt;CB19, "ERROR", "OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="CC35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CD33" s="37" t="str">
+      <c r="CD35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CE33" s="37" t="str">
+      <c r="CE35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CF33" s="37" t="str">
+      <c r="CF35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CG33" s="37" t="str">
+      <c r="CG35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CH33" s="37" t="str">
+      <c r="CH35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CI33" s="37" t="str">
+      <c r="CI35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CJ33" s="37" t="str">
+      <c r="CJ35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CK33" s="37" t="str">
+      <c r="CK35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CL33" s="37" t="str">
+      <c r="CL35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CM33" s="37" t="str">
+      <c r="CM35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CN33" s="37" t="str">
+      <c r="CN35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CO33" s="37" t="str">
+      <c r="CO35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CP33" s="37" t="str">
+      <c r="CP35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CQ33" s="37" t="str">
+      <c r="CQ35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CR33" s="37" t="str">
+      <c r="CR35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CS33" s="37" t="str">
+      <c r="CS35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CT33" s="37" t="str">
+      <c r="CT35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CU33" s="37" t="str">
+      <c r="CU35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CV33" s="37" t="str">
+      <c r="CV35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CW33" s="37" t="str">
+      <c r="CW35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CX33" s="37" t="str">
+      <c r="CX35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CY33" s="37" t="str">
+      <c r="CY35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="CZ33" s="37" t="str">
+      <c r="CZ35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DA33" s="37" t="str">
+      <c r="DA35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DB33" s="37" t="str">
+      <c r="DB35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DC33" s="37" t="str">
+      <c r="DC35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DD33" s="37" t="str">
+      <c r="DD35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DE33" s="37" t="str">
+      <c r="DE35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DF33" s="37" t="str">
+      <c r="DF35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DG33" s="37" t="str">
+      <c r="DG35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DH33" s="37" t="str">
+      <c r="DH35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DI33" s="37" t="str">
+      <c r="DI35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DJ33" s="37" t="str">
+      <c r="DJ35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DK33" s="37" t="str">
+      <c r="DK35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DL33" s="37" t="str">
+      <c r="DL35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DM33" s="37" t="str">
+      <c r="DM35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DN33" s="37" t="str">
+      <c r="DN35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DO33" s="37" t="str">
+      <c r="DO35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DP33" s="37" t="str">
+      <c r="DP35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DQ33" s="37" t="str">
+      <c r="DQ35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DR33" s="37" t="str">
+      <c r="DR35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DS33" s="37" t="str">
+      <c r="DS35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DT33" s="37" t="str">
+      <c r="DT35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DU33" s="37" t="str">
+      <c r="DU35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DV33" s="37" t="str">
+      <c r="DV35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DW33" s="37" t="str">
+      <c r="DW35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DX33" s="37" t="str">
+      <c r="DX35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DY33" s="37" t="str">
+      <c r="DY35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="DZ33" s="37" t="str">
+      <c r="DZ35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EA33" s="37" t="str">
+      <c r="EA35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EB33" s="37" t="str">
+      <c r="EB35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EC33" s="37" t="str">
+      <c r="EC35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="ED33" s="37" t="str">
+      <c r="ED35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EE33" s="37" t="str">
+      <c r="EE35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EF33" s="37" t="str">
+      <c r="EF35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EG33" s="37" t="str">
+      <c r="EG35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EH33" s="37" t="str">
+      <c r="EH35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EI33" s="37" t="str">
+      <c r="EI35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EJ33" s="37" t="str">
+      <c r="EJ35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EK33" s="37" t="str">
+      <c r="EK35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EL33" s="37" t="str">
+      <c r="EL35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EM33" s="37" t="str">
+      <c r="EM35" s="37" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-      <c r="EN33" s="37" t="str">
-        <f t="shared" ref="EN33:FD33" si="3">IF((EN13-0.8)*EN15 &gt;EN17, "ERROR", "OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="EO33" s="37" t="str">
+      <c r="EN35" s="37" t="str">
+        <f t="shared" ref="EN35:FD35" si="3">IF((EN15-0.8)*EN17 &gt;EN19, "ERROR", "OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="EO35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="EP33" s="37" t="str">
+      <c r="EP35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="EQ33" s="37" t="str">
+      <c r="EQ35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="ER33" s="37" t="str">
+      <c r="ER35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="ES33" s="37" t="str">
+      <c r="ES35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="ET33" s="37" t="str">
+      <c r="ET35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="EU33" s="37" t="str">
+      <c r="EU35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="EV33" s="37" t="str">
+      <c r="EV35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="EW33" s="37" t="str">
+      <c r="EW35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="EX33" s="37" t="str">
+      <c r="EX35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="EY33" s="37" t="str">
+      <c r="EY35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="EZ33" s="37" t="str">
+      <c r="EZ35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="FA33" s="37" t="str">
+      <c r="FA35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="FB33" s="37" t="str">
+      <c r="FB35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="FC33" s="37" t="str">
+      <c r="FC35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="FD33" s="37" t="str">
+      <c r="FD35" s="37" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="34" spans="1:160" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="52"/>
-      <c r="B34" s="38" t="s">
+    <row r="36" spans="1:160" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="53"/>
+      <c r="B36" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39" t="str">
-        <f>IF(D18*D20&gt;D21,"ERROR","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="E34" s="39" t="str">
-        <f t="shared" ref="E34:J34" si="4">IF(E18*E20&gt;E21,"ERROR","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="F34" s="39" t="str">
+      <c r="C36" s="39"/>
+      <c r="D36" s="39" t="str">
+        <f>IF(D20*D22&gt;D23,"ERROR","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="E36" s="39" t="str">
+        <f t="shared" ref="E36:J36" si="4">IF(E20*E22&gt;E23,"ERROR","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="F36" s="39" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
-      <c r="G34" s="39" t="str">
+      <c r="G36" s="39" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
-      <c r="H34" s="39" t="str">
+      <c r="H36" s="39" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
-      <c r="I34" s="39" t="str">
+      <c r="I36" s="39" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
-      <c r="J34" s="39" t="str">
+      <c r="J36" s="39" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
-      <c r="K34" s="39" t="str">
-        <f t="shared" ref="K34:O34" si="5">IF(K18*K20&gt;K21,"ERROR","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="L34" s="39" t="str">
+      <c r="K36" s="39" t="str">
+        <f t="shared" ref="K36:O36" si="5">IF(K20*K22&gt;K23,"ERROR","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="L36" s="39" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
       </c>
-      <c r="M34" s="39" t="str">
+      <c r="M36" s="39" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
       </c>
-      <c r="N34" s="39" t="str">
+      <c r="N36" s="39" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
       </c>
-      <c r="O34" s="39" t="str">
+      <c r="O36" s="39" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
       </c>
-      <c r="P34" s="39" t="str">
-        <f t="shared" ref="P34:CA34" si="6">IF(P18*P20&gt;P21,"ERROR","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="Q34" s="39" t="str">
+      <c r="P36" s="39" t="str">
+        <f t="shared" ref="P36:CA36" si="6">IF(P20*P22&gt;P23,"ERROR","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="Q36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="R34" s="39" t="str">
+      <c r="R36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="S34" s="39" t="str">
+      <c r="S36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="T34" s="39" t="str">
+      <c r="T36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="U34" s="39" t="str">
+      <c r="U36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="V34" s="39" t="str">
+      <c r="V36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="W34" s="39" t="str">
+      <c r="W36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="X34" s="39" t="str">
+      <c r="X36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="Y34" s="39" t="str">
+      <c r="Y36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="Z34" s="39" t="str">
+      <c r="Z36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AA34" s="39" t="str">
+      <c r="AA36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AB34" s="39" t="str">
+      <c r="AB36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AC34" s="39" t="str">
+      <c r="AC36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AD34" s="39" t="str">
+      <c r="AD36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AE34" s="39" t="str">
+      <c r="AE36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AF34" s="39" t="str">
+      <c r="AF36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AG34" s="39" t="str">
+      <c r="AG36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AH34" s="39" t="str">
+      <c r="AH36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AI34" s="39" t="str">
+      <c r="AI36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AJ34" s="39" t="str">
+      <c r="AJ36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AK34" s="39" t="str">
+      <c r="AK36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AL34" s="39" t="str">
+      <c r="AL36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AM34" s="39" t="str">
+      <c r="AM36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AN34" s="39" t="str">
+      <c r="AN36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AO34" s="39" t="str">
+      <c r="AO36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AP34" s="39" t="str">
+      <c r="AP36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AQ34" s="39" t="str">
+      <c r="AQ36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AR34" s="39" t="str">
+      <c r="AR36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AS34" s="39" t="str">
+      <c r="AS36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AT34" s="39" t="str">
+      <c r="AT36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AU34" s="39" t="str">
+      <c r="AU36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AV34" s="39" t="str">
+      <c r="AV36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AW34" s="39" t="str">
+      <c r="AW36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AX34" s="39" t="str">
+      <c r="AX36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AY34" s="39" t="str">
+      <c r="AY36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="AZ34" s="39" t="str">
+      <c r="AZ36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BA34" s="39" t="str">
+      <c r="BA36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BB34" s="39" t="str">
+      <c r="BB36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BC34" s="39" t="str">
+      <c r="BC36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BD34" s="39" t="str">
+      <c r="BD36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BE34" s="39" t="str">
+      <c r="BE36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BF34" s="39" t="str">
+      <c r="BF36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BG34" s="39" t="str">
+      <c r="BG36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BH34" s="39" t="str">
+      <c r="BH36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BI34" s="39" t="str">
+      <c r="BI36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BJ34" s="39" t="str">
+      <c r="BJ36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BK34" s="39" t="str">
+      <c r="BK36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BL34" s="39" t="str">
+      <c r="BL36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BM34" s="39" t="str">
+      <c r="BM36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BN34" s="39" t="str">
+      <c r="BN36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BO34" s="39" t="str">
+      <c r="BO36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BP34" s="39" t="str">
+      <c r="BP36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BQ34" s="39" t="str">
+      <c r="BQ36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BR34" s="39" t="str">
+      <c r="BR36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BS34" s="39" t="str">
+      <c r="BS36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BT34" s="39" t="str">
+      <c r="BT36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BU34" s="39" t="str">
+      <c r="BU36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BV34" s="39" t="str">
+      <c r="BV36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BW34" s="39" t="str">
+      <c r="BW36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BX34" s="39" t="str">
+      <c r="BX36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BY34" s="39" t="str">
+      <c r="BY36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="BZ34" s="39" t="str">
+      <c r="BZ36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="CA34" s="39" t="str">
+      <c r="CA36" s="39" t="str">
         <f t="shared" si="6"/>
         <v>OK</v>
       </c>
-      <c r="CB34" s="39" t="str">
-        <f t="shared" ref="CB34:EM34" si="7">IF(CB18*CB20&gt;CB21,"ERROR","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="CC34" s="39" t="str">
+      <c r="CB36" s="39" t="str">
+        <f t="shared" ref="CB36:EM36" si="7">IF(CB20*CB22&gt;CB23,"ERROR","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="CC36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CD34" s="39" t="str">
+      <c r="CD36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CE34" s="39" t="str">
+      <c r="CE36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CF34" s="39" t="str">
+      <c r="CF36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CG34" s="39" t="str">
+      <c r="CG36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CH34" s="39" t="str">
+      <c r="CH36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CI34" s="39" t="str">
+      <c r="CI36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CJ34" s="39" t="str">
+      <c r="CJ36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CK34" s="39" t="str">
+      <c r="CK36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CL34" s="39" t="str">
+      <c r="CL36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CM34" s="39" t="str">
+      <c r="CM36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CN34" s="39" t="str">
+      <c r="CN36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CO34" s="39" t="str">
+      <c r="CO36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CP34" s="39" t="str">
+      <c r="CP36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CQ34" s="39" t="str">
+      <c r="CQ36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CR34" s="39" t="str">
+      <c r="CR36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CS34" s="39" t="str">
+      <c r="CS36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CT34" s="39" t="str">
+      <c r="CT36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CU34" s="39" t="str">
+      <c r="CU36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CV34" s="39" t="str">
+      <c r="CV36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CW34" s="39" t="str">
+      <c r="CW36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CX34" s="39" t="str">
+      <c r="CX36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CY34" s="39" t="str">
+      <c r="CY36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="CZ34" s="39" t="str">
+      <c r="CZ36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DA34" s="39" t="str">
+      <c r="DA36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DB34" s="39" t="str">
+      <c r="DB36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DC34" s="39" t="str">
+      <c r="DC36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DD34" s="39" t="str">
+      <c r="DD36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DE34" s="39" t="str">
+      <c r="DE36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DF34" s="39" t="str">
+      <c r="DF36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DG34" s="39" t="str">
+      <c r="DG36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DH34" s="39" t="str">
+      <c r="DH36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DI34" s="39" t="str">
+      <c r="DI36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DJ34" s="39" t="str">
+      <c r="DJ36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DK34" s="39" t="str">
+      <c r="DK36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DL34" s="39" t="str">
+      <c r="DL36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DM34" s="39" t="str">
+      <c r="DM36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DN34" s="39" t="str">
+      <c r="DN36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DO34" s="39" t="str">
+      <c r="DO36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DP34" s="39" t="str">
+      <c r="DP36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DQ34" s="39" t="str">
+      <c r="DQ36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DR34" s="39" t="str">
+      <c r="DR36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DS34" s="39" t="str">
+      <c r="DS36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DT34" s="39" t="str">
+      <c r="DT36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DU34" s="39" t="str">
+      <c r="DU36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DV34" s="39" t="str">
+      <c r="DV36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DW34" s="39" t="str">
+      <c r="DW36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DX34" s="39" t="str">
+      <c r="DX36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DY34" s="39" t="str">
+      <c r="DY36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="DZ34" s="39" t="str">
+      <c r="DZ36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EA34" s="39" t="str">
+      <c r="EA36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EB34" s="39" t="str">
+      <c r="EB36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EC34" s="39" t="str">
+      <c r="EC36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="ED34" s="39" t="str">
+      <c r="ED36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EE34" s="39" t="str">
+      <c r="EE36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EF34" s="39" t="str">
+      <c r="EF36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EG34" s="39" t="str">
+      <c r="EG36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EH34" s="39" t="str">
+      <c r="EH36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EI34" s="39" t="str">
+      <c r="EI36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EJ34" s="39" t="str">
+      <c r="EJ36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EK34" s="39" t="str">
+      <c r="EK36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EL34" s="39" t="str">
+      <c r="EL36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EM34" s="39" t="str">
+      <c r="EM36" s="39" t="str">
         <f t="shared" si="7"/>
         <v>OK</v>
       </c>
-      <c r="EN34" s="39" t="str">
-        <f t="shared" ref="EN34:FD34" si="8">IF(EN18*EN20&gt;EN21,"ERROR","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="EO34" s="39" t="str">
+      <c r="EN36" s="39" t="str">
+        <f t="shared" ref="EN36:FD36" si="8">IF(EN20*EN22&gt;EN23,"ERROR","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="EO36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="EP34" s="39" t="str">
+      <c r="EP36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="EQ34" s="39" t="str">
+      <c r="EQ36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="ER34" s="39" t="str">
+      <c r="ER36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="ES34" s="39" t="str">
+      <c r="ES36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="ET34" s="39" t="str">
+      <c r="ET36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="EU34" s="39" t="str">
+      <c r="EU36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="EV34" s="39" t="str">
+      <c r="EV36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="EW34" s="39" t="str">
+      <c r="EW36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="EX34" s="39" t="str">
+      <c r="EX36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="EY34" s="39" t="str">
+      <c r="EY36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="EZ34" s="39" t="str">
+      <c r="EZ36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="FA34" s="39" t="str">
+      <c r="FA36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="FB34" s="39" t="str">
+      <c r="FB36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="FC34" s="39" t="str">
+      <c r="FC36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-      <c r="FD34" s="39" t="str">
+      <c r="FD36" s="39" t="str">
         <f t="shared" si="8"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="35" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-    </row>
-    <row r="36" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36"/>
     </row>
     <row r="37" spans="1:160" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37"/>
@@ -16875,34 +17228,40 @@
     </row>
     <row r="1895" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1895"/>
+    </row>
+    <row r="1896" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1896"/>
+    </row>
+    <row r="1897" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1897"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0"/>
   <mergeCells count="3">
     <mergeCell ref="A1:A12"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A13:A32"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A15:A34"/>
   </mergeCells>
-  <conditionalFormatting sqref="D33:FD34">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+  <conditionalFormatting sqref="D35:FD36">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"""OK"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"""ERROR"""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="9">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="FE13:XFD32">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="FE15:XFD34">
       <formula1>0</formula1>
       <formula2>1E+99</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="FE11:XFD12">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="FE11:XFD14">
       <formula1>0</formula1>
       <formula2>1000000000000000000</formula2>
     </dataValidation>
@@ -16922,11 +17281,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:FD4">
       <formula1>rng_rail_material_names</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:FD31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:FD33">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D32:FD32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D34:FD34">
       <formula1>"1,2,4"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>